<commit_message>
test de la clase casilla y mapa , modificaciones en el archivo tablero y en el mapa
</commit_message>
<xml_diff>
--- a/recursos/ejemplo-mapa-mario.xlsx
+++ b/recursos/ejemplo-mapa-mario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>azul: suma o resta monedas</t>
   </si>
@@ -32,14 +32,24 @@
   <si>
     <t>naranja:estrella</t>
   </si>
+  <si>
+    <t>Tablero 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -237,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -265,6 +275,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,13 +297,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -335,13 +347,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -385,13 +397,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>276225</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -435,13 +447,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -485,13 +497,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -535,13 +547,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -585,13 +597,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -635,13 +647,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>361951</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -685,13 +697,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -735,13 +747,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409576</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -785,13 +797,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -835,13 +847,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -885,13 +897,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>390526</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -935,13 +947,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -985,13 +997,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>276226</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1035,13 +1047,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1371,221 +1383,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B3" sqref="B3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1">
+    <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="J1">
+      <c r="J3">
         <v>0</v>
       </c>
-      <c r="K1">
+      <c r="K3">
         <v>1</v>
       </c>
-      <c r="L1">
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="M1">
+      <c r="M3">
         <v>3</v>
       </c>
-      <c r="N1">
+      <c r="N3">
         <v>4</v>
       </c>
-      <c r="O1">
+      <c r="O3">
         <v>5</v>
       </c>
-      <c r="P1">
+      <c r="P3">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="13"/>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="22"/>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="13"/>
       <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="1"/>
       <c r="F5" s="22"/>
       <c r="I5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="15"/>
+      <c r="L5" s="2"/>
       <c r="M5" s="1"/>
       <c r="N5" s="2"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="20"/>
       <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="1"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="1"/>
+      <c r="O6" s="2"/>
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="22"/>
       <c r="I7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="15"/>
       <c r="M7" s="1"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="19"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="12"/>
     </row>
     <row r="8" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="21"/>
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="26"/>
       <c r="I8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="15"/>
       <c r="M8" s="1"/>
       <c r="N8" s="2"/>
       <c r="O8" s="1"/>
       <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
       <c r="I9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="12"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E10" s="21"/>
       <c r="I10">
-        <v>8</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="2"/>
       <c r="O10" s="1"/>
       <c r="P10" s="12"/>
     </row>
     <row r="11" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="21"/>
+        <v>1</v>
+      </c>
       <c r="I11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="2"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
@@ -1593,22 +1580,26 @@
     </row>
     <row r="12" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>10</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="18"/>
       <c r="O12" s="1"/>
       <c r="P12" s="12"/>
     </row>
     <row r="13" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="21"/>
       <c r="I13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="1"/>
@@ -1618,17 +1609,44 @@
       <c r="O13" s="1"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
       <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>11</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I16">
         <v>12</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="11"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agregó un nuevo tablero (tablero3.txt) Se agregó la restricción a la selección de la dirección en las bifurcaciones
</commit_message>
<xml_diff>
--- a/recursos/ejemplo-mapa-mario.xlsx
+++ b/recursos/ejemplo-mapa-mario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4695"/>
+    <workbookView xWindow="480" yWindow="110" windowWidth="14120" windowHeight="4700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>azul: suma o resta monedas</t>
   </si>
@@ -56,7 +56,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,8 +99,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -243,11 +255,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -277,6 +341,20 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,6 +1150,817 @@
         <a:ln w="57150">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>132194</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="17 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="6361545"/>
+          <a:ext cx="1" cy="871104"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>83126</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="27 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9144000" y="6361545"/>
+          <a:ext cx="9525" cy="822036"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="28 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9906000" y="6176818"/>
+          <a:ext cx="819150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="29 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6858000" y="7100455"/>
+          <a:ext cx="447675" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165652</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="19 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="425174" y="281609"/>
+          <a:ext cx="0" cy="248478"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>93869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>49695</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="23 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="425174" y="822739"/>
+          <a:ext cx="0" cy="866913"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>163444</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>86140</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="28 Conector angular"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="425174" y="2070652"/>
+          <a:ext cx="908879" cy="566531"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -1033"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>143566</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>77304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>143566</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="32 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2192131" y="1170608"/>
+          <a:ext cx="0" cy="866913"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>220870</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>93870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>281609</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>93870</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="42 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="806174" y="640522"/>
+          <a:ext cx="938696" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>168966</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>97183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>229705</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>97183</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="45 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2510183" y="1008270"/>
+          <a:ext cx="938696" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>183322</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>100497</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>244061</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>100497</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="46 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2231887" y="2104888"/>
+          <a:ext cx="938696" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>143566</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>82827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>65157</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>87245</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="47 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1899479" y="265044"/>
+          <a:ext cx="1970156" cy="4418"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>106018</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>100496</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>143564</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>100496</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="49 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="691322" y="1922670"/>
+          <a:ext cx="622851" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>143564</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>143564</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104913</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="51 Conector recto de flecha"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3070086" y="2252870"/>
+          <a:ext cx="0" cy="220869"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>5522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160131</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104915</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="54 Conector angular"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3296478" y="1695175"/>
+          <a:ext cx="1010479" cy="911087"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 273"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>160129</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>82827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>220872</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104915</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="62 Conector angular"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3473174" y="828260"/>
+          <a:ext cx="750958" cy="353395"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -1385,11 +2274,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F3"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="27" t="s">
@@ -1636,7 +2525,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I16">
         <v>12</v>
       </c>
@@ -1657,13 +2546,627 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="31">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="18">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="20">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="32">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="35">
+        <v>1</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="18">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="U3" s="39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="38">
+        <v>1</v>
+      </c>
+      <c r="C4" s="33">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="40">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="37"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="33">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="U4" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="37"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="34">
+        <v>1</v>
+      </c>
+      <c r="N5" s="36"/>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="U5" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="38">
+        <v>1</v>
+      </c>
+      <c r="I6" s="33">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="18">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="36"/>
+      <c r="O6" s="20">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="U6" s="30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="35">
+        <v>1</v>
+      </c>
+      <c r="N7" s="36"/>
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="U7" s="41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="18">
+        <v>1</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="36"/>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="22">
+        <v>1</v>
+      </c>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="36"/>
+      <c r="O9" s="22">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="22">
+        <v>1</v>
+      </c>
+      <c r="N10" s="36"/>
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="38">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="34">
+        <v>1</v>
+      </c>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="34">
+        <v>1</v>
+      </c>
+      <c r="N11" s="36"/>
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="42">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="33">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="36"/>
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="34">
+        <v>1</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="34">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="32">
+        <v>1</v>
+      </c>
+      <c r="K15" s="38">
+        <v>1</v>
+      </c>
+      <c r="L15" s="33">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <f>SUM(B2:B15)</f>
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:O16" si="0">SUM(C2:C15)</f>
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1673,7 +3176,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>